<commit_message>
- Modificacion de Alojamiento y Medio CargaArchivos
</commit_message>
<xml_diff>
--- a/Archivos/TR/ARCHIVOS DE CARGA TURISMO RECEPTIVO  SERNATUR V 2.0.xlsx
+++ b/Archivos/TR/ARCHIVOS DE CARGA TURISMO RECEPTIVO  SERNATUR V 2.0.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\CargaDatos\Archivos\TR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\CargaDatos\Archivos\TR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8FDD87-0F91-494D-9122-3E9AC0AD7656}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRIMESTRAL AGR." sheetId="1" r:id="rId1"/>
     <sheet name="DIVISAS" sheetId="2" r:id="rId2"/>
     <sheet name="BASE" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="306">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -245,42 +252,6 @@
   </si>
   <si>
     <t>OPINION</t>
-  </si>
-  <si>
-    <t>Hotel</t>
-  </si>
-  <si>
-    <t>Cabaña</t>
-  </si>
-  <si>
-    <t>Hostal</t>
-  </si>
-  <si>
-    <t>Camping</t>
-  </si>
-  <si>
-    <t>Refugio</t>
-  </si>
-  <si>
-    <t>Lodge</t>
-  </si>
-  <si>
-    <t>Resort</t>
-  </si>
-  <si>
-    <t>depto</t>
-  </si>
-  <si>
-    <t>familia</t>
-  </si>
-  <si>
-    <t>Airbnb</t>
-  </si>
-  <si>
-    <t>crucero</t>
-  </si>
-  <si>
-    <t>otro</t>
   </si>
   <si>
     <t>ALOJAMIENTO</t>
@@ -668,21 +639,12 @@
     <t>Entrevistado</t>
   </si>
   <si>
-    <t>Esposo/pareja</t>
-  </si>
-  <si>
     <t>Hijo(a)/Hijastro(a)</t>
   </si>
   <si>
     <t>Otro familiar</t>
   </si>
   <si>
-    <t>Amigo</t>
-  </si>
-  <si>
-    <t>Compañero de trabajo</t>
-  </si>
-  <si>
     <t>AEROLINEAS ARGENTINAS</t>
   </si>
   <si>
@@ -927,12 +889,90 @@
   </si>
   <si>
     <t>data_tr_base</t>
+  </si>
+  <si>
+    <t>Solo/a</t>
+  </si>
+  <si>
+    <t>Con la pareja/cónyuge</t>
+  </si>
+  <si>
+    <t>Con amigos/as</t>
+  </si>
+  <si>
+    <t>Con compañeros/as de trabajo o estudios</t>
+  </si>
+  <si>
+    <t>Con familiares sin menores de edad</t>
+  </si>
+  <si>
+    <t>Con familiares con menores de edad</t>
+  </si>
+  <si>
+    <t>Acompañado</t>
+  </si>
+  <si>
+    <t>&lt;- AÑO BASE</t>
+  </si>
+  <si>
+    <t>&lt;- AÑO NO BASE</t>
+  </si>
+  <si>
+    <t>Hotel
+/Apart Hotel</t>
+  </si>
+  <si>
+    <t>Cabañas
+/Motel</t>
+  </si>
+  <si>
+    <t>Residencia
+/Hostal</t>
+  </si>
+  <si>
+    <t>Camping
+/Albergue
+/Refugio
+/Lodge
+/Resort (Turístico)</t>
+  </si>
+  <si>
+    <t>Casa
+/Departamento arrendado</t>
+  </si>
+  <si>
+    <t>Airbnb, Couchsurfing, Housetrip</t>
+  </si>
+  <si>
+    <t>Pernoctación 
+en cruceros 
+de bandera chilena</t>
+  </si>
+  <si>
+    <t>Casa de familiares 
+- amigos</t>
+  </si>
+  <si>
+    <t>Residencia 
+particular</t>
+  </si>
+  <si>
+    <t>Recinto 
+particular</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vehículo 
+motorizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Otro. 
+Especifique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -970,7 +1010,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1091,6 +1131,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1128,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1211,9 +1257,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1265,6 +1308,9 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1272,6 +1318,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1310,9 +1359,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1597,7 +1644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1939,7 +1986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2103,11 +2150,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GA41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:GA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BI6" sqref="BI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,7 +2169,7 @@
     <col min="19" max="20" width="15" customWidth="1"/>
     <col min="22" max="22" width="19.85546875" customWidth="1"/>
     <col min="24" max="24" width="16.5703125" customWidth="1"/>
-    <col min="28" max="28" width="14.7109375" style="43" customWidth="1"/>
+    <col min="28" max="28" width="14.7109375" style="42" customWidth="1"/>
     <col min="34" max="34" width="10.5703125" customWidth="1"/>
     <col min="35" max="35" width="11.28515625" customWidth="1"/>
     <col min="36" max="36" width="9.5703125" customWidth="1"/>
@@ -2132,6 +2179,9 @@
     <col min="44" max="44" width="13.28515625" customWidth="1"/>
     <col min="45" max="45" width="13" customWidth="1"/>
     <col min="47" max="47" width="13.140625" customWidth="1"/>
+    <col min="49" max="49" width="11.42578125" customWidth="1"/>
+    <col min="53" max="53" width="11.7109375" customWidth="1"/>
+    <col min="55" max="55" width="12.7109375" customWidth="1"/>
     <col min="61" max="61" width="12.85546875" customWidth="1"/>
     <col min="68" max="68" width="14.5703125" customWidth="1"/>
     <col min="69" max="69" width="13.140625" customWidth="1"/>
@@ -2141,6 +2191,8 @@
     <col min="83" max="85" width="15.28515625" customWidth="1"/>
     <col min="91" max="91" width="12.5703125" customWidth="1"/>
     <col min="92" max="92" width="16.85546875" customWidth="1"/>
+    <col min="97" max="97" width="20.7109375" customWidth="1"/>
+    <col min="98" max="98" width="13.5703125" customWidth="1"/>
     <col min="125" max="125" width="13.7109375" customWidth="1"/>
     <col min="126" max="126" width="17" customWidth="1"/>
     <col min="127" max="127" width="14.28515625" customWidth="1"/>
@@ -2175,7 +2227,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:183" x14ac:dyDescent="0.25">
@@ -2927,13 +2979,13 @@
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
       <c r="J4" s="54" t="s">
         <v>70</v>
       </c>
@@ -2958,13 +3010,13 @@
       <c r="AC4" s="23"/>
       <c r="AD4" s="23"/>
       <c r="AE4" s="23"/>
-      <c r="AF4" s="58" t="s">
+      <c r="AF4" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="AG4" s="58"/>
-      <c r="AH4" s="58"/>
-      <c r="AI4" s="49"/>
-      <c r="AJ4" s="50"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59"/>
+      <c r="AI4" s="48"/>
+      <c r="AJ4" s="49"/>
       <c r="AK4" s="54" t="s">
         <v>6</v>
       </c>
@@ -2972,170 +3024,170 @@
       <c r="AM4" s="54"/>
       <c r="AN4" s="54"/>
       <c r="AO4" s="54"/>
-      <c r="AP4" s="51"/>
-      <c r="AQ4" s="51"/>
-      <c r="AR4" s="57" t="s">
+      <c r="AP4" s="50"/>
+      <c r="AQ4" s="50"/>
+      <c r="AR4" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="AS4" s="57"/>
-      <c r="AT4" s="57"/>
-      <c r="AU4" s="57"/>
+      <c r="AS4" s="58"/>
+      <c r="AT4" s="58"/>
+      <c r="AU4" s="58"/>
       <c r="AV4" s="29"/>
-      <c r="AW4" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="AX4" s="62"/>
-      <c r="AY4" s="62"/>
-      <c r="AZ4" s="62"/>
-      <c r="BA4" s="62"/>
-      <c r="BB4" s="62"/>
-      <c r="BC4" s="62"/>
-      <c r="BD4" s="62"/>
-      <c r="BE4" s="62"/>
-      <c r="BF4" s="62"/>
-      <c r="BG4" s="62"/>
-      <c r="BH4" s="62"/>
-      <c r="BI4" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="BJ4" s="61"/>
-      <c r="BK4" s="61"/>
-      <c r="BL4" s="61"/>
-      <c r="BM4" s="61"/>
-      <c r="BN4" s="61"/>
-      <c r="BO4" s="61"/>
-      <c r="BP4" s="63" t="s">
-        <v>96</v>
-      </c>
-      <c r="BQ4" s="63"/>
-      <c r="BR4" s="63"/>
-      <c r="BS4" s="63"/>
-      <c r="BT4" s="63"/>
-      <c r="BU4" s="63"/>
-      <c r="BV4" s="63"/>
-      <c r="BW4" s="63"/>
-      <c r="BX4" s="63"/>
+      <c r="AW4" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX4" s="63"/>
+      <c r="AY4" s="63"/>
+      <c r="AZ4" s="63"/>
+      <c r="BA4" s="63"/>
+      <c r="BB4" s="63"/>
+      <c r="BC4" s="63"/>
+      <c r="BD4" s="63"/>
+      <c r="BE4" s="63"/>
+      <c r="BF4" s="63"/>
+      <c r="BG4" s="63"/>
+      <c r="BH4" s="63"/>
+      <c r="BI4" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ4" s="62"/>
+      <c r="BK4" s="62"/>
+      <c r="BL4" s="62"/>
+      <c r="BM4" s="62"/>
+      <c r="BN4" s="62"/>
+      <c r="BO4" s="62"/>
+      <c r="BP4" s="64" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ4" s="64"/>
+      <c r="BR4" s="64"/>
+      <c r="BS4" s="64"/>
+      <c r="BT4" s="64"/>
+      <c r="BU4" s="64"/>
+      <c r="BV4" s="64"/>
+      <c r="BW4" s="64"/>
+      <c r="BX4" s="64"/>
       <c r="BY4" s="31"/>
       <c r="BZ4" s="31"/>
-      <c r="CA4" s="64" t="s">
+      <c r="CA4" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="CB4" s="64"/>
-      <c r="CC4" s="64"/>
-      <c r="CD4" s="64"/>
-      <c r="CE4" s="64"/>
-      <c r="CF4" s="64"/>
-      <c r="CG4" s="64"/>
-      <c r="CH4" s="64"/>
-      <c r="CI4" s="64"/>
-      <c r="CJ4" s="64"/>
-      <c r="CK4" s="64"/>
-      <c r="CL4" s="64"/>
-      <c r="CM4" s="64"/>
-      <c r="CN4" s="64"/>
-      <c r="CO4" s="64"/>
-      <c r="CP4" s="65" t="s">
+      <c r="CB4" s="65"/>
+      <c r="CC4" s="65"/>
+      <c r="CD4" s="65"/>
+      <c r="CE4" s="65"/>
+      <c r="CF4" s="65"/>
+      <c r="CG4" s="65"/>
+      <c r="CH4" s="65"/>
+      <c r="CI4" s="65"/>
+      <c r="CJ4" s="65"/>
+      <c r="CK4" s="65"/>
+      <c r="CL4" s="65"/>
+      <c r="CM4" s="65"/>
+      <c r="CN4" s="65"/>
+      <c r="CO4" s="65"/>
+      <c r="CP4" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="CQ4" s="65"/>
-      <c r="CR4" s="65"/>
-      <c r="CS4" s="65"/>
-      <c r="CT4" s="65"/>
-      <c r="CU4" s="65"/>
-      <c r="CV4" s="65"/>
-      <c r="CW4" s="65"/>
-      <c r="CX4" s="65"/>
-      <c r="CY4" s="65"/>
-      <c r="CZ4" s="65"/>
-      <c r="DA4" s="65"/>
-      <c r="DB4" s="65"/>
-      <c r="DC4" s="65"/>
-      <c r="DD4" s="65"/>
-      <c r="DE4" s="65"/>
-      <c r="DF4" s="65"/>
-      <c r="DG4" s="65"/>
-      <c r="DH4" s="65"/>
-      <c r="DI4" s="65"/>
-      <c r="DJ4" s="65"/>
-      <c r="DK4" s="65"/>
-      <c r="DL4" s="65"/>
-      <c r="DM4" s="65"/>
-      <c r="DN4" s="65"/>
-      <c r="DO4" s="65"/>
-      <c r="DP4" s="65"/>
-      <c r="DQ4" s="65"/>
-      <c r="DR4" s="65"/>
+      <c r="CQ4" s="66"/>
+      <c r="CR4" s="66"/>
+      <c r="CS4" s="66"/>
+      <c r="CT4" s="66"/>
+      <c r="CU4" s="66"/>
+      <c r="CV4" s="66"/>
+      <c r="CW4" s="66"/>
+      <c r="CX4" s="66"/>
+      <c r="CY4" s="66"/>
+      <c r="CZ4" s="66"/>
+      <c r="DA4" s="66"/>
+      <c r="DB4" s="66"/>
+      <c r="DC4" s="66"/>
+      <c r="DD4" s="66"/>
+      <c r="DE4" s="66"/>
+      <c r="DF4" s="66"/>
+      <c r="DG4" s="66"/>
+      <c r="DH4" s="66"/>
+      <c r="DI4" s="66"/>
+      <c r="DJ4" s="66"/>
+      <c r="DK4" s="66"/>
+      <c r="DL4" s="66"/>
+      <c r="DM4" s="66"/>
+      <c r="DN4" s="66"/>
+      <c r="DO4" s="66"/>
+      <c r="DP4" s="66"/>
+      <c r="DQ4" s="66"/>
+      <c r="DR4" s="66"/>
       <c r="DS4" s="30"/>
-      <c r="DT4" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="DU4" s="66"/>
-      <c r="DV4" s="66"/>
-      <c r="DW4" s="66"/>
-      <c r="DX4" s="66"/>
-      <c r="DY4" s="66"/>
-      <c r="DZ4" s="66"/>
-      <c r="EA4" s="66"/>
-      <c r="EB4" s="66"/>
-      <c r="EC4" s="66"/>
-      <c r="ED4" s="66"/>
-      <c r="EE4" s="66"/>
-      <c r="EF4" s="66"/>
-      <c r="EG4" s="66"/>
-      <c r="EH4" s="66"/>
-      <c r="EI4" s="66"/>
-      <c r="EJ4" s="66"/>
-      <c r="EK4" s="66"/>
-      <c r="EL4" s="66"/>
-      <c r="EM4" s="66"/>
-      <c r="EN4" s="66"/>
-      <c r="EO4" s="66"/>
-      <c r="EP4" s="66"/>
-      <c r="EQ4" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="ER4" s="59"/>
-      <c r="ES4" s="59"/>
-      <c r="ET4" s="59"/>
-      <c r="EU4" s="59"/>
-      <c r="EV4" s="59"/>
-      <c r="EW4" s="59"/>
-      <c r="EX4" s="59"/>
-      <c r="EY4" s="59"/>
-      <c r="EZ4" s="59"/>
-      <c r="FA4" s="59"/>
-      <c r="FB4" s="60" t="s">
-        <v>182</v>
-      </c>
-      <c r="FC4" s="60"/>
-      <c r="FD4" s="60"/>
-      <c r="FE4" s="60"/>
-      <c r="FF4" s="60"/>
-      <c r="FG4" s="60"/>
-      <c r="FH4" s="60"/>
-      <c r="FI4" s="60"/>
-      <c r="FJ4" s="60"/>
-      <c r="FK4" s="60"/>
-      <c r="FL4" s="60"/>
-      <c r="FM4" s="60"/>
-      <c r="FN4" s="60"/>
-      <c r="FO4" s="60"/>
-      <c r="FP4" s="61" t="s">
-        <v>187</v>
-      </c>
-      <c r="FQ4" s="61"/>
-      <c r="FR4" s="61"/>
-      <c r="FS4" s="61"/>
-      <c r="FT4" s="61"/>
-      <c r="FU4" s="55" t="s">
-        <v>204</v>
-      </c>
-      <c r="FV4" s="55"/>
-      <c r="FW4" s="55"/>
-      <c r="FX4" s="55"/>
-      <c r="FY4" s="55"/>
-      <c r="FZ4" s="55"/>
-      <c r="GA4" s="55"/>
+      <c r="DT4" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="DU4" s="67"/>
+      <c r="DV4" s="67"/>
+      <c r="DW4" s="67"/>
+      <c r="DX4" s="67"/>
+      <c r="DY4" s="67"/>
+      <c r="DZ4" s="67"/>
+      <c r="EA4" s="67"/>
+      <c r="EB4" s="67"/>
+      <c r="EC4" s="67"/>
+      <c r="ED4" s="67"/>
+      <c r="EE4" s="67"/>
+      <c r="EF4" s="67"/>
+      <c r="EG4" s="67"/>
+      <c r="EH4" s="67"/>
+      <c r="EI4" s="67"/>
+      <c r="EJ4" s="67"/>
+      <c r="EK4" s="67"/>
+      <c r="EL4" s="67"/>
+      <c r="EM4" s="67"/>
+      <c r="EN4" s="67"/>
+      <c r="EO4" s="67"/>
+      <c r="EP4" s="67"/>
+      <c r="EQ4" s="60" t="s">
+        <v>156</v>
+      </c>
+      <c r="ER4" s="60"/>
+      <c r="ES4" s="60"/>
+      <c r="ET4" s="60"/>
+      <c r="EU4" s="60"/>
+      <c r="EV4" s="60"/>
+      <c r="EW4" s="60"/>
+      <c r="EX4" s="60"/>
+      <c r="EY4" s="60"/>
+      <c r="EZ4" s="60"/>
+      <c r="FA4" s="60"/>
+      <c r="FB4" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="FC4" s="61"/>
+      <c r="FD4" s="61"/>
+      <c r="FE4" s="61"/>
+      <c r="FF4" s="61"/>
+      <c r="FG4" s="61"/>
+      <c r="FH4" s="61"/>
+      <c r="FI4" s="61"/>
+      <c r="FJ4" s="61"/>
+      <c r="FK4" s="61"/>
+      <c r="FL4" s="61"/>
+      <c r="FM4" s="61"/>
+      <c r="FN4" s="61"/>
+      <c r="FO4" s="61"/>
+      <c r="FP4" s="62" t="s">
+        <v>175</v>
+      </c>
+      <c r="FQ4" s="62"/>
+      <c r="FR4" s="62"/>
+      <c r="FS4" s="62"/>
+      <c r="FT4" s="62"/>
+      <c r="FU4" s="56" t="s">
+        <v>192</v>
+      </c>
+      <c r="FV4" s="56"/>
+      <c r="FW4" s="56"/>
+      <c r="FX4" s="56"/>
+      <c r="FY4" s="56"/>
+      <c r="FZ4" s="56"/>
+      <c r="GA4" s="56"/>
     </row>
     <row r="5" spans="1:183" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -3160,7 +3212,7 @@
         <v>43</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="11" t="s">
@@ -3186,34 +3238,34 @@
         <v>20</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="U5" s="26" t="s">
         <v>49</v>
       </c>
       <c r="V5" s="26"/>
-      <c r="W5" s="42" t="s">
-        <v>205</v>
-      </c>
-      <c r="X5" s="42"/>
-      <c r="Y5" s="42" t="s">
-        <v>206</v>
-      </c>
-      <c r="Z5" s="42" t="s">
-        <v>207</v>
-      </c>
-      <c r="AA5" s="44" t="s">
-        <v>208</v>
-      </c>
-      <c r="AB5" s="44"/>
-      <c r="AC5" s="44" t="s">
-        <v>209</v>
-      </c>
-      <c r="AD5" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="AE5" s="45" t="s">
-        <v>211</v>
+      <c r="W5" s="41" t="s">
+        <v>193</v>
+      </c>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z5" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA5" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD5" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE5" s="44" t="s">
+        <v>199</v>
       </c>
       <c r="AF5" s="25" t="s">
         <v>46</v>
@@ -3224,10 +3276,10 @@
       <c r="AH5" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="AI5" s="48" t="s">
-        <v>256</v>
-      </c>
-      <c r="AJ5" s="48" t="s">
+      <c r="AI5" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="AJ5" s="47" t="s">
         <v>21</v>
       </c>
       <c r="AK5" s="11" t="s">
@@ -3244,10 +3296,10 @@
       </c>
       <c r="AO5" s="11"/>
       <c r="AP5" s="11" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="AQ5" s="11" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="AR5" s="9" t="s">
         <v>52</v>
@@ -3260,484 +3312,484 @@
       <c r="AV5" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="AW5" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX5" s="32" t="s">
+      <c r="AW5" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="AX5" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="AY5" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="AZ5" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BA5" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="BB5" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="BC5" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="BD5" s="25" t="s">
+        <v>301</v>
+      </c>
+      <c r="BE5" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="BF5" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="BG5" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="BH5" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="BI5" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="BJ5" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="BK5" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL5" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="BM5" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="BN5" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="BO5" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="AY5" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="AZ5" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="BA5" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="BB5" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="BC5" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="BD5" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="BE5" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="BF5" s="32" t="s">
+      <c r="BP5" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="BG5" s="32" t="s">
+      <c r="BQ5" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="BH5" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="BI5" s="33" t="s">
+      <c r="BR5" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="BS5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="BT5" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="BU5" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="BJ5" s="33" t="s">
+      <c r="BV5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="BW5" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="BK5" s="33" t="s">
+      <c r="BX5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="BY5" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="BZ5" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="CA5" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="CB5" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="CC5" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="CD5" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="CE5" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="CF5" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="CG5" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="CH5" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="BL5" s="33" t="s">
+      <c r="CI5" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="CJ5" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="CK5" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="CL5" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="CM5" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="CN5" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="CO5" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="BM5" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="BN5" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="BO5" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="BP5" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="BQ5" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="BR5" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="BS5" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="BT5" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="BU5" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="BV5" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="BW5" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="BX5" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="BY5" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="BZ5" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="CA5" s="34" t="s">
+      <c r="CP5" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="CQ5" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="CB5" s="34" t="s">
+      <c r="CR5" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="CS5" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="CC5" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="CD5" s="34" t="s">
+      <c r="CT5" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="CE5" s="34" t="s">
+      <c r="CU5" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="CV5" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="CW5" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="CX5" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="CY5" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="CF5" s="34" t="s">
+      <c r="CZ5" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="CG5" s="34" t="s">
+      <c r="DA5" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="DB5" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="CH5" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="CI5" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="CJ5" s="34" t="s">
+      <c r="DC5" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="DD5" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="DE5" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="DF5" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="CK5" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="CL5" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="CM5" s="34" t="s">
+      <c r="DG5" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="DH5" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="CN5" s="34" t="s">
+      <c r="DI5" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="CO5" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="CP5" s="33" t="s">
+      <c r="DJ5" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="DK5" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="CQ5" s="33" t="s">
+      <c r="DL5" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="CR5" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="CS5" s="35" t="s">
+      <c r="DM5" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="DN5" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="CT5" s="35" t="s">
+      <c r="DO5" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="CU5" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="CV5" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="CW5" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="CX5" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="CY5" s="35" t="s">
+      <c r="DP5" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="DQ5" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="CZ5" s="35" t="s">
+      <c r="DR5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="DA5" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="DB5" s="33" t="s">
+      <c r="DS5" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="DT5" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="DC5" s="33" t="s">
+      <c r="DU5" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="DV5" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="DD5" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="DE5" s="35" t="s">
+      <c r="DW5" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="DF5" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="DG5" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="DH5" s="33" t="s">
+      <c r="DX5" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="DI5" s="33" t="s">
+      <c r="DY5" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="DJ5" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="DK5" s="35" t="s">
+      <c r="DZ5" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="DL5" s="35" t="s">
+      <c r="EA5" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="DM5" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="DN5" s="33" t="s">
+      <c r="EB5" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="DO5" s="33" t="s">
+      <c r="EC5" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="DP5" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="DQ5" s="35" t="s">
+      <c r="ED5" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="DR5" s="35" t="s">
+      <c r="EE5" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="DS5" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="DT5" s="24" t="s">
+      <c r="EF5" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="DU5" s="24" t="s">
+      <c r="EG5" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="DV5" s="24" t="s">
+      <c r="EH5" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="DW5" s="24" t="s">
+      <c r="EI5" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="DX5" s="24" t="s">
+      <c r="EJ5" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="DY5" s="24" t="s">
+      <c r="EK5" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="DZ5" s="24" t="s">
+      <c r="EL5" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="EA5" s="24" t="s">
+      <c r="EM5" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="EB5" s="24" t="s">
+      <c r="EN5" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="EC5" s="24" t="s">
+      <c r="EO5" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="ED5" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="EE5" s="24" t="s">
+      <c r="EP5" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="EQ5" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="EF5" s="24" t="s">
+      <c r="ER5" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="EG5" s="24" t="s">
+      <c r="ES5" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="EH5" s="24" t="s">
+      <c r="ET5" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="EU5" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="EI5" s="24" t="s">
+      <c r="EV5" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="EJ5" s="24" t="s">
+      <c r="EW5" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="EK5" s="24" t="s">
+      <c r="EX5" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="EL5" s="24" t="s">
+      <c r="EY5" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="EM5" s="24" t="s">
+      <c r="EZ5" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="EN5" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="EO5" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="EP5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="EQ5" s="36" t="s">
+      <c r="FA5" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="FB5" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="FC5" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="ER5" s="36" t="s">
+      <c r="FD5" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="ES5" s="36" t="s">
+      <c r="FE5" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="ET5" s="36" t="s">
+      <c r="FF5" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="FG5" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="FH5" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="FI5" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="FJ5" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="FK5" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="FL5" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="FM5" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="EU5" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="EV5" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="EW5" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="EX5" s="36" t="s">
-        <v>165</v>
-      </c>
-      <c r="EY5" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="EZ5" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="FA5" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="FB5" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="FC5" s="9" t="s">
+      <c r="FN5" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="FO5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="FP5" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="FD5" s="9" t="s">
+      <c r="FQ5" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="FE5" s="9" t="s">
+      <c r="FR5" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="FF5" s="9" t="s">
+      <c r="FS5" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="FG5" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="FH5" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="FI5" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="FJ5" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="FK5" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="FL5" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="FM5" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="FN5" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="FO5" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="FP5" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="FQ5" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="FR5" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="FS5" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="FT5" s="33" t="s">
-        <v>86</v>
+      <c r="FT5" s="32" t="s">
+        <v>74</v>
       </c>
       <c r="FU5" s="26" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="FV5" s="26" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="FW5" s="26" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="FX5" s="26" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="FY5" s="26" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="FZ5" s="26" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="GA5" s="26" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:183" s="12" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="36">
         <v>2018</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="36">
         <v>3</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="36">
         <v>31</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="37">
         <v>2.51911614201806E+22</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="36">
         <v>2585</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="37">
+      <c r="H6" s="36">
         <v>1520100</v>
       </c>
-      <c r="I6" s="37" t="s">
-        <v>257</v>
-      </c>
-      <c r="J6" s="37">
+      <c r="I6" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="J6" s="36">
         <v>1304</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="37">
+      <c r="L6" s="36">
         <v>1304</v>
       </c>
-      <c r="M6" s="37" t="s">
+      <c r="M6" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="37">
-        <v>1</v>
-      </c>
-      <c r="P6" s="37" t="s">
+      <c r="O6" s="36">
+        <v>1</v>
+      </c>
+      <c r="P6" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="Q6" s="37">
-        <v>1</v>
-      </c>
-      <c r="R6" s="37" t="s">
+      <c r="Q6" s="36">
+        <v>1</v>
+      </c>
+      <c r="R6" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="S6" s="37">
+      <c r="S6" s="36">
         <v>4</v>
       </c>
-      <c r="T6" s="37">
-        <v>1</v>
-      </c>
-      <c r="U6" s="39">
-        <v>1</v>
-      </c>
-      <c r="V6" s="39" t="s">
-        <v>188</v>
+      <c r="T6" s="36">
+        <v>1</v>
+      </c>
+      <c r="U6" s="38">
+        <v>1</v>
+      </c>
+      <c r="V6" s="38" t="s">
+        <v>176</v>
       </c>
       <c r="W6" s="28">
         <v>4</v>
       </c>
       <c r="X6" s="28" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="Y6" s="28">
         <v>201</v>
@@ -3745,11 +3797,11 @@
       <c r="Z6" s="28">
         <v>500</v>
       </c>
-      <c r="AA6" s="46">
+      <c r="AA6" s="45">
         <v>2</v>
       </c>
-      <c r="AB6" s="47" t="s">
-        <v>219</v>
+      <c r="AB6" s="46" t="s">
+        <v>204</v>
       </c>
       <c r="AC6" s="28">
         <v>201</v>
@@ -3760,55 +3812,55 @@
       <c r="AE6" s="28">
         <v>1250.5</v>
       </c>
-      <c r="AF6" s="40">
+      <c r="AF6" s="39">
         <v>2</v>
       </c>
-      <c r="AG6" s="40">
+      <c r="AG6" s="39">
         <v>3</v>
       </c>
-      <c r="AH6" s="40">
+      <c r="AH6" s="39">
         <v>5</v>
       </c>
-      <c r="AI6" s="41">
+      <c r="AI6" s="40">
         <v>332.65</v>
       </c>
-      <c r="AJ6" s="40">
+      <c r="AJ6" s="39">
         <v>20</v>
       </c>
-      <c r="AK6" s="41">
+      <c r="AK6" s="40">
         <v>1015.18</v>
       </c>
-      <c r="AL6" s="41">
+      <c r="AL6" s="40">
         <v>1015.18</v>
       </c>
-      <c r="AM6" s="41">
+      <c r="AM6" s="40">
         <v>50.75</v>
       </c>
-      <c r="AN6" s="39">
+      <c r="AN6" s="38">
         <v>3</v>
       </c>
-      <c r="AO6" s="39" t="s">
+      <c r="AO6" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="AP6" s="37">
+      <c r="AP6" s="36">
         <v>1184.8</v>
       </c>
-      <c r="AQ6" s="37">
+      <c r="AQ6" s="36">
         <v>1974.67</v>
       </c>
-      <c r="AR6" s="41">
-        <v>1</v>
-      </c>
-      <c r="AS6" s="37" t="s">
+      <c r="AR6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AS6" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AT6" s="37">
-        <v>1</v>
-      </c>
-      <c r="AU6" s="37" t="s">
+      <c r="AT6" s="36">
+        <v>1</v>
+      </c>
+      <c r="AU6" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="AV6" s="37">
+      <c r="AV6" s="36">
         <v>61.11</v>
       </c>
       <c r="AW6" s="12">
@@ -3896,16 +3948,16 @@
         <v>0</v>
       </c>
       <c r="BY6" s="12" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="BZ6" s="12" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="CA6" s="28">
         <v>1500</v>
       </c>
       <c r="CB6" s="28" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="CC6" s="28">
         <v>597.15</v>
@@ -4264,7 +4316,7 @@
         <v>14</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="U7" s="13" t="s">
         <v>14</v>
@@ -4335,88 +4387,88 @@
         <v>16</v>
       </c>
       <c r="AW7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="AX7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="AY7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="AZ7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BA7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BB7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BC7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BD7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BE7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BF7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BG7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BH7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BI7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BJ7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BK7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BL7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BM7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BN7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BO7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BP7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BQ7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BR7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BS7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BT7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BU7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BV7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BW7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BX7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="BY7" s="13" t="s">
         <v>15</v>
@@ -4540,184 +4592,184 @@
       </c>
       <c r="DS7" s="13"/>
       <c r="DT7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="DU7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="DV7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="DW7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="DX7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="DY7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="DZ7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EA7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EB7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EC7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="ED7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EE7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EF7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EG7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EH7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EI7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EJ7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EK7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EL7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EM7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EN7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EO7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EP7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EQ7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="ER7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="ES7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="ET7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EU7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EV7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EW7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EX7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EY7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="EZ7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FA7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FB7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FC7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FD7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FE7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FF7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FG7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FH7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FI7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FJ7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FK7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FL7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FM7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FN7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FO7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FP7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FQ7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FR7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FS7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FT7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FU7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FV7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FW7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FX7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FY7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="FZ7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="GA7" s="13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:183" x14ac:dyDescent="0.25">
@@ -5175,546 +5227,546 @@
     </row>
     <row r="9" spans="1:183" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>299</v>
-      </c>
-      <c r="B9" s="67" t="s">
+        <v>284</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>253</v>
+      </c>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" t="s">
+        <v>252</v>
+      </c>
+      <c r="F9" t="s">
+        <v>254</v>
+      </c>
+      <c r="G9" t="s">
+        <v>255</v>
+      </c>
+      <c r="H9" t="s">
+        <v>256</v>
+      </c>
+      <c r="I9" t="s">
+        <v>257</v>
+      </c>
+      <c r="J9" t="s">
+        <v>259</v>
+      </c>
+      <c r="K9" t="s">
+        <v>257</v>
+      </c>
+      <c r="L9" t="s">
+        <v>258</v>
+      </c>
+      <c r="M9" t="s">
+        <v>257</v>
+      </c>
+      <c r="N9" t="s">
+        <v>260</v>
+      </c>
+      <c r="O9" t="s">
+        <v>261</v>
+      </c>
+      <c r="P9" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>257</v>
+      </c>
+      <c r="R9" t="s">
+        <v>257</v>
+      </c>
+      <c r="S9" t="s">
+        <v>262</v>
+      </c>
+      <c r="T9" t="s">
+        <v>263</v>
+      </c>
+      <c r="U9" t="s">
+        <v>264</v>
+      </c>
+      <c r="V9" t="s">
+        <v>257</v>
+      </c>
+      <c r="W9" t="s">
+        <v>265</v>
+      </c>
+      <c r="X9" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>266</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>267</v>
+      </c>
+      <c r="AA9" t="s">
         <v>268</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" t="s">
-        <v>267</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="AB9" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="AC9" t="s">
         <v>269</v>
       </c>
-      <c r="G9" t="s">
+      <c r="AD9" t="s">
         <v>270</v>
       </c>
-      <c r="H9" t="s">
+      <c r="AF9" t="s">
         <v>271</v>
       </c>
-      <c r="I9" t="s">
+      <c r="AG9" t="s">
         <v>272</v>
       </c>
-      <c r="J9" t="s">
+      <c r="AH9" t="s">
+        <v>273</v>
+      </c>
+      <c r="AI9" t="s">
         <v>274</v>
       </c>
-      <c r="K9" t="s">
-        <v>272</v>
-      </c>
-      <c r="L9" t="s">
-        <v>273</v>
-      </c>
-      <c r="M9" t="s">
-        <v>272</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="AJ9" t="s">
         <v>275</v>
       </c>
-      <c r="O9" t="s">
+      <c r="AK9" t="s">
         <v>276</v>
       </c>
-      <c r="P9" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>272</v>
-      </c>
-      <c r="R9" t="s">
-        <v>272</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="AL9" t="s">
         <v>277</v>
       </c>
-      <c r="T9" t="s">
+      <c r="AM9" t="s">
         <v>278</v>
       </c>
-      <c r="U9" t="s">
+      <c r="AN9" t="s">
         <v>279</v>
       </c>
-      <c r="V9" t="s">
-        <v>272</v>
-      </c>
-      <c r="W9" t="s">
+      <c r="AO9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AR9" t="s">
         <v>280</v>
       </c>
-      <c r="X9" t="s">
-        <v>272</v>
-      </c>
-      <c r="Y9" t="s">
+      <c r="AS9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AT9" t="s">
         <v>281</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AU9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BG9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BJ9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BK9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BL9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BM9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BN9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BO9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BP9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BQ9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BR9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BS9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BT9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BU9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BV9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BW9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BX9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BY9" t="s">
         <v>282</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="BZ9" t="s">
         <v>283</v>
       </c>
-      <c r="AB9" s="43" t="s">
-        <v>272</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>284</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>285</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>286</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>287</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>288</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>289</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>290</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>291</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>292</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>293</v>
-      </c>
-      <c r="AN9" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>272</v>
-      </c>
-      <c r="AP9" t="s">
-        <v>272</v>
-      </c>
-      <c r="AQ9" t="s">
-        <v>272</v>
-      </c>
-      <c r="AR9" t="s">
-        <v>295</v>
-      </c>
-      <c r="AS9" t="s">
-        <v>272</v>
-      </c>
-      <c r="AT9" t="s">
-        <v>296</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>272</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>272</v>
-      </c>
-      <c r="AW9" t="s">
-        <v>272</v>
-      </c>
-      <c r="AX9" t="s">
-        <v>272</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>272</v>
-      </c>
-      <c r="AZ9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BA9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BB9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BC9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BE9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BF9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BG9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BH9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BI9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BJ9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BK9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BL9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BM9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BN9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BO9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BP9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BQ9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BR9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BS9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BT9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BU9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BV9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BW9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BX9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BY9" t="s">
-        <v>297</v>
-      </c>
-      <c r="BZ9" t="s">
-        <v>298</v>
-      </c>
       <c r="CA9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CB9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CC9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CD9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CE9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CF9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CG9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CH9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CI9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CJ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CK9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CL9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CM9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CN9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CO9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CP9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CQ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CR9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CS9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CT9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CU9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CV9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CW9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CX9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CY9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="CZ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DA9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DB9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DC9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DD9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DE9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DF9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DG9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DH9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DI9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DJ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DK9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DL9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DM9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DN9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DO9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DP9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DQ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DR9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DS9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DT9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DU9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DV9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DW9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DX9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DY9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="DZ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EA9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EB9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EC9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="ED9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EE9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EF9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EG9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EH9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EI9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EJ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EK9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EL9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EM9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EN9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EO9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EP9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EQ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="ER9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="ES9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="ET9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EU9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EV9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EW9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EX9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EY9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="EZ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FA9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FB9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FC9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FD9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FE9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FF9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FG9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FH9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FI9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FJ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FK9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FL9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FM9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FN9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FO9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FP9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FQ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FR9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FS9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FT9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FU9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FV9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FW9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FX9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FY9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="FZ9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="GA9" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:183" x14ac:dyDescent="0.25">
@@ -5722,24 +5774,24 @@
         <v>49</v>
       </c>
       <c r="W10" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:183" x14ac:dyDescent="0.25">
       <c r="T11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="U11">
         <v>1</v>
       </c>
       <c r="V11" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="W11">
         <v>1</v>
       </c>
       <c r="X11" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="AN11">
         <v>1</v>
@@ -5760,37 +5812,37 @@
         <v>59</v>
       </c>
       <c r="AW11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="BI11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="BP11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="CA11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="CP11" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="CR11" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="DT11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="EQ11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="FB11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="FP11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="FU11" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:183" x14ac:dyDescent="0.25">
@@ -5798,19 +5850,19 @@
         <v>27</v>
       </c>
       <c r="T12" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="U12">
         <v>2</v>
       </c>
       <c r="V12" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="W12">
         <v>2</v>
       </c>
       <c r="X12" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="AN12">
         <v>2</v>
@@ -5831,43 +5883,43 @@
         <v>60</v>
       </c>
       <c r="AW12" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="BI12" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="BP12" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="CA12" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="CP12">
         <v>1</v>
       </c>
       <c r="CQ12" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="CR12">
         <v>1</v>
       </c>
       <c r="CS12" t="s">
-        <v>212</v>
+        <v>285</v>
       </c>
       <c r="DT12" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="EQ12" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="FB12" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="FP12" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="FU12" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:183" x14ac:dyDescent="0.25">
@@ -5878,13 +5930,13 @@
         <v>3</v>
       </c>
       <c r="V13" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="W13">
         <v>3</v>
       </c>
       <c r="X13" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="AN13">
         <v>3</v>
@@ -5908,331 +5960,365 @@
         <v>2</v>
       </c>
       <c r="CQ13" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="CR13">
         <v>2</v>
       </c>
       <c r="CS13" t="s">
-        <v>213</v>
+        <v>286</v>
+      </c>
+      <c r="CT13" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:183" x14ac:dyDescent="0.25">
-      <c r="U14">
-        <v>4</v>
-      </c>
-      <c r="V14" t="s">
-        <v>191</v>
-      </c>
-      <c r="W14">
-        <v>4</v>
-      </c>
-      <c r="X14" t="s">
-        <v>221</v>
-      </c>
-      <c r="AN14">
-        <v>4</v>
-      </c>
-      <c r="AO14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AR14">
-        <v>4</v>
-      </c>
-      <c r="AS14" t="s">
-        <v>57</v>
-      </c>
-      <c r="AT14">
-        <v>4</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>57</v>
-      </c>
-      <c r="CR14">
-        <v>3</v>
-      </c>
-      <c r="CS14" t="s">
-        <v>214</v>
+      <c r="AB14" s="51"/>
+      <c r="CR14" s="68">
+        <v>2</v>
+      </c>
+      <c r="CS14" s="68" t="s">
+        <v>291</v>
+      </c>
+      <c r="CT14" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:183" x14ac:dyDescent="0.25">
       <c r="U15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V15" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="W15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X15" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="AN15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AO15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AR15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AS15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AT15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CR15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="CS15" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:183" x14ac:dyDescent="0.25">
       <c r="U16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V16" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="W16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X16" t="s">
-        <v>223</v>
+        <v>207</v>
+      </c>
+      <c r="AN16">
+        <v>5</v>
+      </c>
+      <c r="AO16" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR16">
+        <v>5</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT16">
+        <v>5</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>58</v>
       </c>
       <c r="CR16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CS16" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="21:97" x14ac:dyDescent="0.25">
       <c r="U17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V17" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="W17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X17" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="CR17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="CS17" t="s">
-        <v>217</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="21:97" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>7</v>
+      </c>
+      <c r="V18" t="s">
+        <v>182</v>
+      </c>
       <c r="W18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X18" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="CR18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="CS18" t="s">
-        <v>86</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W19">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X19" t="s">
-        <v>226</v>
+        <v>210</v>
+      </c>
+      <c r="CR19">
+        <v>7</v>
+      </c>
+      <c r="CS19" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W20">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="X20" t="s">
-        <v>227</v>
+        <v>211</v>
+      </c>
+      <c r="CR20">
+        <v>8</v>
+      </c>
+      <c r="CS20" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W21">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X21" t="s">
-        <v>228</v>
+        <v>212</v>
+      </c>
+      <c r="CR21">
+        <v>9</v>
+      </c>
+      <c r="CS21" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W22">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X22" t="s">
-        <v>229</v>
+        <v>213</v>
+      </c>
+      <c r="CR22">
+        <v>10</v>
+      </c>
+      <c r="CS22" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W23">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X23" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W24">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X24" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W25">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="X25" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W26">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="X26" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W27">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="X27" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W28">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="X28" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W29">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="X29" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W30">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="X30" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W31">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X31" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="21:97" x14ac:dyDescent="0.25">
       <c r="W32">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X32" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="23:24" x14ac:dyDescent="0.25">
       <c r="W33">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X33" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="23:24" x14ac:dyDescent="0.25">
       <c r="W34">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="X34" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="23:24" x14ac:dyDescent="0.25">
       <c r="W35">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="X35" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="23:24" x14ac:dyDescent="0.25">
       <c r="W36">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="X36" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="23:24" x14ac:dyDescent="0.25">
       <c r="W37">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X37" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="23:24" x14ac:dyDescent="0.25">
       <c r="W38">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X38" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="23:24" x14ac:dyDescent="0.25">
       <c r="W39">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X39" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="23:24" x14ac:dyDescent="0.25">
       <c r="W40">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X40" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="23:24" x14ac:dyDescent="0.25">
       <c r="W41">
+        <v>30</v>
+      </c>
+      <c r="X41" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="23:24" x14ac:dyDescent="0.25">
+      <c r="W42">
         <v>99</v>
       </c>
-      <c r="X41" t="s">
-        <v>248</v>
+      <c r="X42" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="DT4:EP4"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="FU4:GA4"/>
     <mergeCell ref="AK4:AO4"/>
@@ -6249,7 +6335,6 @@
     <mergeCell ref="BP4:BX4"/>
     <mergeCell ref="CA4:CO4"/>
     <mergeCell ref="CP4:DR4"/>
-    <mergeCell ref="DT4:EP4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>